<commit_message>
Se han añadido cosas a los objetivos
+ objetivos
+ referencias
</commit_message>
<xml_diff>
--- a/Entregables/ChangeLog.xlsx
+++ b/Entregables/ChangeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Cambios</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Se hizo un primer esbozo de los objetivos y el planning</t>
+  </si>
+  <si>
+    <t>Retoque de los objetivos, se han añadido cosas</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +507,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
elaboracion de la estructura y ideas principales
</commit_message>
<xml_diff>
--- a/Entregables/ChangeLog.xlsx
+++ b/Entregables/ChangeLog.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="11190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="11190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Informe Inicial" sheetId="1" r:id="rId1"/>
+    <sheet name="Primer informe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Cambios</t>
   </si>
@@ -60,6 +61,12 @@
   </si>
   <si>
     <t>Acabando el informe final</t>
+  </si>
+  <si>
+    <t>PRIMER INFORME</t>
+  </si>
+  <si>
+    <t>elaboracion de la estructura e ideas principales</t>
   </si>
 </sst>
 </file>
@@ -477,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,4 +595,86 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="50.42578125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>43204</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>43204</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correcciones coen + other
+ correccion coen
+ creacion del indice
+ creacion del archivo de dependencias
+ creacion del archivo
</commit_message>
<xml_diff>
--- a/Entregables/ChangeLog.xlsx
+++ b/Entregables/ChangeLog.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="11190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="11190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Informe Inicial" sheetId="1" r:id="rId1"/>
     <sheet name="Primer informe" sheetId="2" r:id="rId2"/>
+    <sheet name="Segundo informe" sheetId="3" r:id="rId3"/>
+    <sheet name="Informe Final" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Cambios</t>
   </si>
@@ -76,6 +78,105 @@
   </si>
   <si>
     <t>se añaden las secciones de development progress y se desarrollan</t>
+  </si>
+  <si>
+    <t>Informe final acabado</t>
+  </si>
+  <si>
+    <t>SEGUNDO INFORME</t>
+  </si>
+  <si>
+    <t>Informe Final</t>
+  </si>
+  <si>
+    <t>retoques en el desarrollo, cambios en el planning y retoques en dataset</t>
+  </si>
+  <si>
+    <t>actualizado arbol de tareas</t>
+  </si>
+  <si>
+    <t>actualizado gantt</t>
+  </si>
+  <si>
+    <t>se han añadido imagenes</t>
+  </si>
+  <si>
+    <t>version final, algunas correcciones</t>
+  </si>
+  <si>
+    <t>añadido progresso del desarrollo i cambios en la intro</t>
+  </si>
+  <si>
+    <t>se han añadido referencias y modificado el planning</t>
+  </si>
+  <si>
+    <t>ligeras modificaciones y correciones</t>
+  </si>
+  <si>
+    <t>se añade la seccion de user testing y se modifica la metodologia</t>
+  </si>
+  <si>
+    <t>correcciones</t>
+  </si>
+  <si>
+    <t>version final</t>
+  </si>
+  <si>
+    <t>creacion del documento</t>
+  </si>
+  <si>
+    <t>se planea y se crea la estructura del documento</t>
+  </si>
+  <si>
+    <t>se reestructura el documento despues de la reunion</t>
+  </si>
+  <si>
+    <t>se añade la metodologia y los objetivos</t>
+  </si>
+  <si>
+    <t>se añade la introduccion y el state of the art</t>
+  </si>
+  <si>
+    <t>correccion ortografica</t>
+  </si>
+  <si>
+    <t>se añade la seccion de desarrollo de libelas</t>
+  </si>
+  <si>
+    <t>se han añadido las explicaciones sobre los efectos de la distancia</t>
+  </si>
+  <si>
+    <t>añadido user testing y revisado todo el texto</t>
+  </si>
+  <si>
+    <t>se han añadido las graficas del user testing</t>
+  </si>
+  <si>
+    <t>se ha modificado la explicacion del pipeline</t>
+  </si>
+  <si>
+    <t>añadidas las explicaciones de la segunda session de user testing y el protocolo del user testing</t>
+  </si>
+  <si>
+    <t>añadidas projectos futuros y agradecimientos</t>
+  </si>
+  <si>
+    <t>añadidas las conclusiones y añadidas imágenes epipolares</t>
+  </si>
+  <si>
+    <t>coreccion ortografica</t>
+  </si>
+  <si>
+    <t>añadida explicacion sobre el output de libelas</t>
+  </si>
+  <si>
+    <t>revision general y correcciones varias</t>
+  </si>
+  <si>
+    <t>creacion del abstract</t>
+  </si>
+  <si>
+    <t>añadidos resultados de roi</t>
   </si>
 </sst>
 </file>
@@ -166,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -177,6 +278,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +701,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>43170</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
@@ -608,10 +720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,16 +795,44 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+      <c r="B10" s="6">
+        <v>43208</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <v>43208</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <v>43208</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <v>43208</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>43210</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -701,4 +841,299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="57.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>43242</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>43243</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>43244</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>43244</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>43245</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>43246</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>43247</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="86.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>43268</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>43268</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>43269</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>43269</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>43271</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>43272</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>43272</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>43274</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>43276</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>43276</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>43276</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>43276</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>43277</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>43278</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>43278</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>43279</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>43280</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>43280</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>43280</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>43280</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>